<commit_message>
High score skærm og alt der tilhører den og så dagens burndown chart
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f4ad920445e6980/Dokumenter/Digital design/DDU---Projekt---Platformspil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{02857FE0-5529-4C80-9ED0-0993D0CCC8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B691C8B6-557C-40AC-B419-FA54ED799867}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{02857FE0-5529-4C80-9ED0-0993D0CCC8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50BF4A83-3C91-4F87-B052-FF4D8F3CEE24}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3AC0DAFF-710F-44E4-A74A-CE4400C2B976}"/>
   </bookViews>
@@ -223,7 +223,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1435,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B6769D-47E3-40D7-8E6C-7239BB802F95}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1467,13 +1467,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1490,6 +1490,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Knap og  burndown chart
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f4ad920445e6980/Dokumenter/Digital design/DDU---Projekt---Platformspil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{02857FE0-5529-4C80-9ED0-0993D0CCC8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50BF4A83-3C91-4F87-B052-FF4D8F3CEE24}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{02857FE0-5529-4C80-9ED0-0993D0CCC8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{558C4A49-B888-4786-903B-5516603B2CEF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3AC0DAFF-710F-44E4-A74A-CE4400C2B976}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>Tid(t)</t>
   </si>
   <si>
-    <t>Antal tasks</t>
+    <t>Antal tasks tilbage</t>
   </si>
 </sst>
 </file>
@@ -223,7 +223,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1435,17 +1435,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B6769D-47E3-40D7-8E6C-7239BB802F95}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" customWidth="1"/>
     <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1467,13 +1467,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1487,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1495,7 +1495,23 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
burndown chart er nu færdig
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonat\Documents\GitHub\DDU---Projekt---Platformspil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f4ad920445e6980/Dokumenter/Digital design/DDU---Projekt---Platformspil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AA2DED-481E-43BE-B4E6-CDC374FB0441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{C6AA2DED-481E-43BE-B4E6-CDC374FB0441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7416DCF1-8750-4F0D-878E-90598DC63F33}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2320" windowWidth="14400" windowHeight="7360" xr2:uid="{3AC0DAFF-710F-44E4-A74A-CE4400C2B976}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3AC0DAFF-710F-44E4-A74A-CE4400C2B976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t>Antal tasks tilbage</t>
   </si>
   <si>
-    <t>?</t>
+    <t>summeret tid()</t>
   </si>
 </sst>
 </file>
@@ -105,7 +105,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -167,19 +167,32 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12548381452318461"/>
+          <c:y val="0.15319444444444447"/>
+          <c:w val="0.83129396325459315"/>
+          <c:h val="0.51681284631087776"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Det ideelle forløb</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -234,14 +247,124 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A2E-40EB-BCED-798052FB8E02}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Det reelle forløb</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7F1B-4914-B126-54150FFDC2CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -303,8 +426,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.47672790901137357"/>
-              <c:y val="0.87868037328667248"/>
+              <c:x val="0.48228346456692911"/>
+              <c:y val="0.75831000291630213"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -332,7 +455,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="da-DK"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -370,7 +493,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="553567776"/>
@@ -454,7 +577,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="da-DK"/>
+              <a:endParaRPr lang="en-DK"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -492,7 +615,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="553571104"/>
@@ -507,6 +630,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32567147856517931"/>
+          <c:y val="0.8524300087489064"/>
+          <c:w val="0.57218591426071741"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -533,7 +697,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1105,15 +1269,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1142,7 +1306,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1438,17 +1602,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B6769D-47E3-40D7-8E6C-7239BB802F95}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" customWidth="1"/>
     <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1462,6 +1627,9 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1476,6 +1644,10 @@
         <v>0</v>
       </c>
       <c r="D2">
+        <f>C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>10</v>
       </c>
     </row>
@@ -1490,6 +1662,10 @@
         <v>6</v>
       </c>
       <c r="D3">
+        <f>C3+D2</f>
+        <v>6</v>
+      </c>
+      <c r="E3">
         <v>8</v>
       </c>
     </row>
@@ -1498,6 +1674,10 @@
         <v>9</v>
       </c>
       <c r="D4">
+        <f t="shared" ref="D4:D10" si="0">C4+D3</f>
+        <v>15</v>
+      </c>
+      <c r="E4">
         <v>6</v>
       </c>
     </row>
@@ -1506,6 +1686,10 @@
         <v>6</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E5">
         <v>6</v>
       </c>
     </row>
@@ -1514,6 +1698,10 @@
         <v>6</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
     </row>
@@ -1522,9 +1710,10 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E7">
         <v>3</v>
       </c>
     </row>
@@ -1533,6 +1722,10 @@
         <v>4</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E8">
         <v>0</v>
       </c>
     </row>
@@ -1541,7 +1734,23 @@
         <v>2</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E9">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>